<commit_message>
possibility to set mpc control period
</commit_message>
<xml_diff>
--- a/EMS_simulation/data_input/energy_sell_price_10min_granularity.xlsx
+++ b/EMS_simulation/data_input/energy_sell_price_10min_granularity.xlsx
@@ -128,10 +128,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1153"/>
+  <dimension ref="A1:B722"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1150" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1161" activeCellId="0" sqref="L1161"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A706" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A722" activeCellId="0" sqref="722:1154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5908,3462 +5908,439 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="722" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A722" s="1" t="n">
-        <v>43226.0000000032</v>
-      </c>
-      <c r="B722" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="723" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A723" s="1" t="n">
-        <v>43226.0069444477</v>
-      </c>
-      <c r="B723" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="724" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A724" s="1" t="n">
-        <v>43226.0138888921</v>
-      </c>
-      <c r="B724" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="725" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A725" s="1" t="n">
-        <v>43226.0208333366</v>
-      </c>
-      <c r="B725" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="726" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A726" s="1" t="n">
-        <v>43226.027777781</v>
-      </c>
-      <c r="B726" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="727" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A727" s="1" t="n">
-        <v>43226.0347222255</v>
-      </c>
-      <c r="B727" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="728" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A728" s="1" t="n">
-        <v>43226.0416666699</v>
-      </c>
-      <c r="B728" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="729" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A729" s="1" t="n">
-        <v>43226.0486111144</v>
-      </c>
-      <c r="B729" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="730" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A730" s="1" t="n">
-        <v>43226.0555555588</v>
-      </c>
-      <c r="B730" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="731" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A731" s="1" t="n">
-        <v>43226.0625000033</v>
-      </c>
-      <c r="B731" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="732" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A732" s="1" t="n">
-        <v>43226.0694444477</v>
-      </c>
-      <c r="B732" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="733" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A733" s="1" t="n">
-        <v>43226.0763888922</v>
-      </c>
-      <c r="B733" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="734" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A734" s="1" t="n">
-        <v>43226.0833333366</v>
-      </c>
-      <c r="B734" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="735" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A735" s="1" t="n">
-        <v>43226.0902777811</v>
-      </c>
-      <c r="B735" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="736" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A736" s="1" t="n">
-        <v>43226.0972222255</v>
-      </c>
-      <c r="B736" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="737" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A737" s="1" t="n">
-        <v>43226.10416667</v>
-      </c>
-      <c r="B737" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="738" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A738" s="1" t="n">
-        <v>43226.1111111144</v>
-      </c>
-      <c r="B738" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="739" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A739" s="1" t="n">
-        <v>43226.1180555589</v>
-      </c>
-      <c r="B739" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="740" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A740" s="1" t="n">
-        <v>43226.1250000033</v>
-      </c>
-      <c r="B740" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="741" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A741" s="1" t="n">
-        <v>43226.1319444478</v>
-      </c>
-      <c r="B741" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="742" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A742" s="1" t="n">
-        <v>43226.1388888922</v>
-      </c>
-      <c r="B742" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="743" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A743" s="1" t="n">
-        <v>43226.1458333367</v>
-      </c>
-      <c r="B743" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="744" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A744" s="1" t="n">
-        <v>43226.1527777811</v>
-      </c>
-      <c r="B744" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="745" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A745" s="1" t="n">
-        <v>43226.1597222256</v>
-      </c>
-      <c r="B745" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="746" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A746" s="1" t="n">
-        <v>43226.16666667</v>
-      </c>
-      <c r="B746" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="747" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A747" s="1" t="n">
-        <v>43226.1736111145</v>
-      </c>
-      <c r="B747" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="748" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A748" s="1" t="n">
-        <v>43226.1805555589</v>
-      </c>
-      <c r="B748" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="749" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A749" s="1" t="n">
-        <v>43226.1875000034</v>
-      </c>
-      <c r="B749" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="750" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A750" s="1" t="n">
-        <v>43226.1944444478</v>
-      </c>
-      <c r="B750" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="751" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A751" s="1" t="n">
-        <v>43226.2013888923</v>
-      </c>
-      <c r="B751" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="752" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A752" s="1" t="n">
-        <v>43226.2083333367</v>
-      </c>
-      <c r="B752" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="753" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A753" s="1" t="n">
-        <v>43226.2152777812</v>
-      </c>
-      <c r="B753" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="754" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A754" s="1" t="n">
-        <v>43226.2222222256</v>
-      </c>
-      <c r="B754" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="755" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A755" s="1" t="n">
-        <v>43226.2291666701</v>
-      </c>
-      <c r="B755" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="756" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A756" s="1" t="n">
-        <v>43226.2361111145</v>
-      </c>
-      <c r="B756" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="757" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A757" s="1" t="n">
-        <v>43226.243055559</v>
-      </c>
-      <c r="B757" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="758" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A758" s="1" t="n">
-        <v>43226.2500000034</v>
-      </c>
-      <c r="B758" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="759" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A759" s="1" t="n">
-        <v>43226.2569444479</v>
-      </c>
-      <c r="B759" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="760" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A760" s="1" t="n">
-        <v>43226.2638888923</v>
-      </c>
-      <c r="B760" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="761" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A761" s="1" t="n">
-        <v>43226.2708333368</v>
-      </c>
-      <c r="B761" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="762" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A762" s="1" t="n">
-        <v>43226.2777777812</v>
-      </c>
-      <c r="B762" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="763" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A763" s="1" t="n">
-        <v>43226.2847222257</v>
-      </c>
-      <c r="B763" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="764" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A764" s="1" t="n">
-        <v>43226.2916666701</v>
-      </c>
-      <c r="B764" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="765" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A765" s="1" t="n">
-        <v>43226.2986111146</v>
-      </c>
-      <c r="B765" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="766" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A766" s="1" t="n">
-        <v>43226.305555559</v>
-      </c>
-      <c r="B766" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="767" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A767" s="1" t="n">
-        <v>43226.3125000035</v>
-      </c>
-      <c r="B767" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="768" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A768" s="1" t="n">
-        <v>43226.3194444479</v>
-      </c>
-      <c r="B768" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="769" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A769" s="1" t="n">
-        <v>43226.3263888924</v>
-      </c>
-      <c r="B769" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="770" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A770" s="1" t="n">
-        <v>43226.3333333368</v>
-      </c>
-      <c r="B770" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="771" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A771" s="1" t="n">
-        <v>43226.3402777813</v>
-      </c>
-      <c r="B771" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="772" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A772" s="1" t="n">
-        <v>43226.3472222257</v>
-      </c>
-      <c r="B772" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="773" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A773" s="1" t="n">
-        <v>43226.3541666702</v>
-      </c>
-      <c r="B773" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="774" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A774" s="1" t="n">
-        <v>43226.3611111146</v>
-      </c>
-      <c r="B774" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="775" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A775" s="1" t="n">
-        <v>43226.3680555591</v>
-      </c>
-      <c r="B775" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="776" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A776" s="1" t="n">
-        <v>43226.3750000035</v>
-      </c>
-      <c r="B776" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="777" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A777" s="1" t="n">
-        <v>43226.381944448</v>
-      </c>
-      <c r="B777" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="778" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A778" s="1" t="n">
-        <v>43226.3888888924</v>
-      </c>
-      <c r="B778" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="779" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A779" s="1" t="n">
-        <v>43226.3958333369</v>
-      </c>
-      <c r="B779" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="780" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A780" s="1" t="n">
-        <v>43226.4027777813</v>
-      </c>
-      <c r="B780" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="781" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A781" s="1" t="n">
-        <v>43226.4097222258</v>
-      </c>
-      <c r="B781" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="782" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A782" s="1" t="n">
-        <v>43226.4166666702</v>
-      </c>
-      <c r="B782" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="783" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A783" s="1" t="n">
-        <v>43226.4236111147</v>
-      </c>
-      <c r="B783" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="784" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A784" s="1" t="n">
-        <v>43226.4305555591</v>
-      </c>
-      <c r="B784" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="785" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A785" s="1" t="n">
-        <v>43226.4375000036</v>
-      </c>
-      <c r="B785" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="786" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A786" s="1" t="n">
-        <v>43226.444444448</v>
-      </c>
-      <c r="B786" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="787" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A787" s="1" t="n">
-        <v>43226.4513888925</v>
-      </c>
-      <c r="B787" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="788" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A788" s="1" t="n">
-        <v>43226.4583333369</v>
-      </c>
-      <c r="B788" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="789" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A789" s="1" t="n">
-        <v>43226.4652777814</v>
-      </c>
-      <c r="B789" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="790" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A790" s="1" t="n">
-        <v>43226.4722222258</v>
-      </c>
-      <c r="B790" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="791" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A791" s="1" t="n">
-        <v>43226.4791666703</v>
-      </c>
-      <c r="B791" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="792" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A792" s="1" t="n">
-        <v>43226.4861111147</v>
-      </c>
-      <c r="B792" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="793" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A793" s="1" t="n">
-        <v>43226.4930555592</v>
-      </c>
-      <c r="B793" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="794" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A794" s="1" t="n">
-        <v>43226.5000000036</v>
-      </c>
-      <c r="B794" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="795" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A795" s="1" t="n">
-        <v>43226.5069444481</v>
-      </c>
-      <c r="B795" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="796" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A796" s="1" t="n">
-        <v>43226.5138888925</v>
-      </c>
-      <c r="B796" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="797" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A797" s="1" t="n">
-        <v>43226.520833337</v>
-      </c>
-      <c r="B797" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="798" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A798" s="1" t="n">
-        <v>43226.5277777814</v>
-      </c>
-      <c r="B798" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="799" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A799" s="1" t="n">
-        <v>43226.5347222259</v>
-      </c>
-      <c r="B799" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="800" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A800" s="1" t="n">
-        <v>43226.5416666703</v>
-      </c>
-      <c r="B800" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="801" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A801" s="1" t="n">
-        <v>43226.5486111148</v>
-      </c>
-      <c r="B801" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="802" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A802" s="1" t="n">
-        <v>43226.5555555592</v>
-      </c>
-      <c r="B802" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="803" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A803" s="1" t="n">
-        <v>43226.5625000037</v>
-      </c>
-      <c r="B803" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="804" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A804" s="1" t="n">
-        <v>43226.5694444481</v>
-      </c>
-      <c r="B804" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="805" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A805" s="1" t="n">
-        <v>43226.5763888926</v>
-      </c>
-      <c r="B805" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="806" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A806" s="1" t="n">
-        <v>43226.583333337</v>
-      </c>
-      <c r="B806" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="807" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A807" s="1" t="n">
-        <v>43226.5902777815</v>
-      </c>
-      <c r="B807" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="808" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A808" s="1" t="n">
-        <v>43226.5972222259</v>
-      </c>
-      <c r="B808" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="809" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A809" s="1" t="n">
-        <v>43226.6041666704</v>
-      </c>
-      <c r="B809" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="810" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A810" s="1" t="n">
-        <v>43226.6111111148</v>
-      </c>
-      <c r="B810" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="811" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A811" s="1" t="n">
-        <v>43226.6180555593</v>
-      </c>
-      <c r="B811" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="812" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A812" s="1" t="n">
-        <v>43226.6250000037</v>
-      </c>
-      <c r="B812" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="813" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A813" s="1" t="n">
-        <v>43226.6319444482</v>
-      </c>
-      <c r="B813" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="814" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A814" s="1" t="n">
-        <v>43226.6388888926</v>
-      </c>
-      <c r="B814" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="815" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A815" s="1" t="n">
-        <v>43226.6458333371</v>
-      </c>
-      <c r="B815" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="816" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A816" s="1" t="n">
-        <v>43226.6527777815</v>
-      </c>
-      <c r="B816" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="817" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A817" s="1" t="n">
-        <v>43226.659722226</v>
-      </c>
-      <c r="B817" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="818" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A818" s="1" t="n">
-        <v>43226.6666666704</v>
-      </c>
-      <c r="B818" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="819" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A819" s="1" t="n">
-        <v>43226.6736111149</v>
-      </c>
-      <c r="B819" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="820" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A820" s="1" t="n">
-        <v>43226.6805555593</v>
-      </c>
-      <c r="B820" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="821" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A821" s="1" t="n">
-        <v>43226.6875000038</v>
-      </c>
-      <c r="B821" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="822" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A822" s="1" t="n">
-        <v>43226.6944444482</v>
-      </c>
-      <c r="B822" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="823" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A823" s="1" t="n">
-        <v>43226.7013888927</v>
-      </c>
-      <c r="B823" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="824" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A824" s="1" t="n">
-        <v>43226.7083333371</v>
-      </c>
-      <c r="B824" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="825" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A825" s="1" t="n">
-        <v>43226.7152777816</v>
-      </c>
-      <c r="B825" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="826" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A826" s="1" t="n">
-        <v>43226.722222226</v>
-      </c>
-      <c r="B826" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="827" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A827" s="1" t="n">
-        <v>43226.7291666705</v>
-      </c>
-      <c r="B827" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="828" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A828" s="1" t="n">
-        <v>43226.7361111149</v>
-      </c>
-      <c r="B828" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="829" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A829" s="1" t="n">
-        <v>43226.7430555594</v>
-      </c>
-      <c r="B829" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="830" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A830" s="1" t="n">
-        <v>43226.7500000038</v>
-      </c>
-      <c r="B830" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="831" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A831" s="1" t="n">
-        <v>43226.7569444483</v>
-      </c>
-      <c r="B831" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="832" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A832" s="1" t="n">
-        <v>43226.7638888927</v>
-      </c>
-      <c r="B832" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="833" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A833" s="1" t="n">
-        <v>43226.7708333372</v>
-      </c>
-      <c r="B833" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="834" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A834" s="1" t="n">
-        <v>43226.7777777816</v>
-      </c>
-      <c r="B834" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="835" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A835" s="1" t="n">
-        <v>43226.7847222261</v>
-      </c>
-      <c r="B835" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="836" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A836" s="1" t="n">
-        <v>43226.7916666705</v>
-      </c>
-      <c r="B836" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="837" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A837" s="1" t="n">
-        <v>43226.798611115</v>
-      </c>
-      <c r="B837" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="838" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A838" s="1" t="n">
-        <v>43226.8055555594</v>
-      </c>
-      <c r="B838" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="839" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A839" s="1" t="n">
-        <v>43226.8125000039</v>
-      </c>
-      <c r="B839" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="840" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A840" s="1" t="n">
-        <v>43226.8194444483</v>
-      </c>
-      <c r="B840" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="841" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A841" s="1" t="n">
-        <v>43226.8263888928</v>
-      </c>
-      <c r="B841" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="842" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A842" s="1" t="n">
-        <v>43226.8333333372</v>
-      </c>
-      <c r="B842" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="843" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A843" s="1" t="n">
-        <v>43226.8402777817</v>
-      </c>
-      <c r="B843" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="844" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A844" s="1" t="n">
-        <v>43226.8472222261</v>
-      </c>
-      <c r="B844" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="845" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A845" s="1" t="n">
-        <v>43226.8541666706</v>
-      </c>
-      <c r="B845" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="846" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A846" s="1" t="n">
-        <v>43226.861111115</v>
-      </c>
-      <c r="B846" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="847" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A847" s="1" t="n">
-        <v>43226.8680555595</v>
-      </c>
-      <c r="B847" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="848" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A848" s="1" t="n">
-        <v>43226.8750000039</v>
-      </c>
-      <c r="B848" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="849" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A849" s="1" t="n">
-        <v>43226.8819444484</v>
-      </c>
-      <c r="B849" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="850" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A850" s="1" t="n">
-        <v>43226.8888888928</v>
-      </c>
-      <c r="B850" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="851" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A851" s="1" t="n">
-        <v>43226.8958333373</v>
-      </c>
-      <c r="B851" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="852" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A852" s="1" t="n">
-        <v>43226.9027777817</v>
-      </c>
-      <c r="B852" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="853" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A853" s="1" t="n">
-        <v>43226.9097222262</v>
-      </c>
-      <c r="B853" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="854" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A854" s="1" t="n">
-        <v>43226.9166666706</v>
-      </c>
-      <c r="B854" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="855" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A855" s="1" t="n">
-        <v>43226.9236111151</v>
-      </c>
-      <c r="B855" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="856" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A856" s="1" t="n">
-        <v>43226.9305555595</v>
-      </c>
-      <c r="B856" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="857" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A857" s="1" t="n">
-        <v>43226.937500004</v>
-      </c>
-      <c r="B857" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="858" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A858" s="1" t="n">
-        <v>43226.9444444484</v>
-      </c>
-      <c r="B858" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="859" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A859" s="1" t="n">
-        <v>43226.9513888929</v>
-      </c>
-      <c r="B859" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="860" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A860" s="1" t="n">
-        <v>43226.9583333373</v>
-      </c>
-      <c r="B860" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="861" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A861" s="1" t="n">
-        <v>43226.9652777818</v>
-      </c>
-      <c r="B861" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="862" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A862" s="1" t="n">
-        <v>43226.9722222262</v>
-      </c>
-      <c r="B862" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="863" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A863" s="1" t="n">
-        <v>43226.9791666707</v>
-      </c>
-      <c r="B863" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="864" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A864" s="1" t="n">
-        <v>43226.9861111151</v>
-      </c>
-      <c r="B864" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="865" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A865" s="1" t="n">
-        <v>43226.9930555596</v>
-      </c>
-      <c r="B865" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="866" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A866" s="1" t="n">
-        <v>43227.000000004</v>
-      </c>
-      <c r="B866" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="867" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A867" s="1" t="n">
-        <v>43227.0069444485</v>
-      </c>
-      <c r="B867" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="868" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A868" s="1" t="n">
-        <v>43227.0138888929</v>
-      </c>
-      <c r="B868" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="869" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A869" s="1" t="n">
-        <v>43227.0208333374</v>
-      </c>
-      <c r="B869" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="870" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A870" s="1" t="n">
-        <v>43227.0277777818</v>
-      </c>
-      <c r="B870" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="871" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A871" s="1" t="n">
-        <v>43227.0347222263</v>
-      </c>
-      <c r="B871" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="872" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A872" s="1" t="n">
-        <v>43227.0416666707</v>
-      </c>
-      <c r="B872" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="873" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A873" s="1" t="n">
-        <v>43227.0486111152</v>
-      </c>
-      <c r="B873" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="874" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A874" s="1" t="n">
-        <v>43227.0555555596</v>
-      </c>
-      <c r="B874" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="875" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A875" s="1" t="n">
-        <v>43227.0625000041</v>
-      </c>
-      <c r="B875" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="876" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A876" s="1" t="n">
-        <v>43227.0694444485</v>
-      </c>
-      <c r="B876" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="877" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A877" s="1" t="n">
-        <v>43227.076388893</v>
-      </c>
-      <c r="B877" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="878" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A878" s="1" t="n">
-        <v>43227.0833333374</v>
-      </c>
-      <c r="B878" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="879" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A879" s="1" t="n">
-        <v>43227.0902777819</v>
-      </c>
-      <c r="B879" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="880" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A880" s="1" t="n">
-        <v>43227.0972222263</v>
-      </c>
-      <c r="B880" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="881" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A881" s="1" t="n">
-        <v>43227.1041666708</v>
-      </c>
-      <c r="B881" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="882" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A882" s="1" t="n">
-        <v>43227.1111111152</v>
-      </c>
-      <c r="B882" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="883" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A883" s="1" t="n">
-        <v>43227.1180555597</v>
-      </c>
-      <c r="B883" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="884" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A884" s="1" t="n">
-        <v>43227.1250000041</v>
-      </c>
-      <c r="B884" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="885" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A885" s="1" t="n">
-        <v>43227.1319444486</v>
-      </c>
-      <c r="B885" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="886" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A886" s="1" t="n">
-        <v>43227.138888893</v>
-      </c>
-      <c r="B886" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="887" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A887" s="1" t="n">
-        <v>43227.1458333375</v>
-      </c>
-      <c r="B887" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="888" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A888" s="1" t="n">
-        <v>43227.1527777819</v>
-      </c>
-      <c r="B888" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="889" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A889" s="1" t="n">
-        <v>43227.1597222264</v>
-      </c>
-      <c r="B889" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="890" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A890" s="1" t="n">
-        <v>43227.1666666708</v>
-      </c>
-      <c r="B890" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="891" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A891" s="1" t="n">
-        <v>43227.1736111153</v>
-      </c>
-      <c r="B891" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="892" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A892" s="1" t="n">
-        <v>43227.1805555597</v>
-      </c>
-      <c r="B892" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="893" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A893" s="1" t="n">
-        <v>43227.1875000042</v>
-      </c>
-      <c r="B893" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="894" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A894" s="1" t="n">
-        <v>43227.1944444486</v>
-      </c>
-      <c r="B894" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="895" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A895" s="1" t="n">
-        <v>43227.2013888931</v>
-      </c>
-      <c r="B895" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="896" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A896" s="1" t="n">
-        <v>43227.2083333375</v>
-      </c>
-      <c r="B896" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="897" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A897" s="1" t="n">
-        <v>43227.215277782</v>
-      </c>
-      <c r="B897" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="898" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A898" s="1" t="n">
-        <v>43227.2222222264</v>
-      </c>
-      <c r="B898" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="899" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A899" s="1" t="n">
-        <v>43227.2291666709</v>
-      </c>
-      <c r="B899" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="900" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A900" s="1" t="n">
-        <v>43227.2361111153</v>
-      </c>
-      <c r="B900" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="901" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A901" s="1" t="n">
-        <v>43227.2430555598</v>
-      </c>
-      <c r="B901" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="902" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A902" s="1" t="n">
-        <v>43227.2500000042</v>
-      </c>
-      <c r="B902" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="903" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A903" s="1" t="n">
-        <v>43227.2569444487</v>
-      </c>
-      <c r="B903" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="904" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A904" s="1" t="n">
-        <v>43227.2638888931</v>
-      </c>
-      <c r="B904" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="905" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A905" s="1" t="n">
-        <v>43227.2708333376</v>
-      </c>
-      <c r="B905" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="906" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A906" s="1" t="n">
-        <v>43227.277777782</v>
-      </c>
-      <c r="B906" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="907" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A907" s="1" t="n">
-        <v>43227.2847222265</v>
-      </c>
-      <c r="B907" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="908" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A908" s="1" t="n">
-        <v>43227.2916666709</v>
-      </c>
-      <c r="B908" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="909" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A909" s="1" t="n">
-        <v>43227.2986111154</v>
-      </c>
-      <c r="B909" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="910" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A910" s="1" t="n">
-        <v>43227.3055555598</v>
-      </c>
-      <c r="B910" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="911" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A911" s="1" t="n">
-        <v>43227.3125000043</v>
-      </c>
-      <c r="B911" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="912" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A912" s="1" t="n">
-        <v>43227.3194444487</v>
-      </c>
-      <c r="B912" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="913" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A913" s="1" t="n">
-        <v>43227.3263888932</v>
-      </c>
-      <c r="B913" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="914" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A914" s="1" t="n">
-        <v>43227.3333333376</v>
-      </c>
-      <c r="B914" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="915" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A915" s="1" t="n">
-        <v>43227.3402777821</v>
-      </c>
-      <c r="B915" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="916" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A916" s="1" t="n">
-        <v>43227.3472222265</v>
-      </c>
-      <c r="B916" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="917" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A917" s="1" t="n">
-        <v>43227.354166671</v>
-      </c>
-      <c r="B917" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="918" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A918" s="1" t="n">
-        <v>43227.3611111154</v>
-      </c>
-      <c r="B918" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="919" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A919" s="1" t="n">
-        <v>43227.3680555599</v>
-      </c>
-      <c r="B919" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="920" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A920" s="1" t="n">
-        <v>43227.3750000043</v>
-      </c>
-      <c r="B920" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="921" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A921" s="1" t="n">
-        <v>43227.3819444488</v>
-      </c>
-      <c r="B921" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="922" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A922" s="1" t="n">
-        <v>43227.3888888932</v>
-      </c>
-      <c r="B922" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="923" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A923" s="1" t="n">
-        <v>43227.3958333377</v>
-      </c>
-      <c r="B923" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="924" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A924" s="1" t="n">
-        <v>43227.4027777821</v>
-      </c>
-      <c r="B924" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="925" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A925" s="1" t="n">
-        <v>43227.4097222266</v>
-      </c>
-      <c r="B925" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="926" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A926" s="1" t="n">
-        <v>43227.416666671</v>
-      </c>
-      <c r="B926" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="927" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A927" s="1" t="n">
-        <v>43227.4236111155</v>
-      </c>
-      <c r="B927" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="928" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A928" s="1" t="n">
-        <v>43227.4305555599</v>
-      </c>
-      <c r="B928" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="929" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A929" s="1" t="n">
-        <v>43227.4375000044</v>
-      </c>
-      <c r="B929" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="930" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A930" s="1" t="n">
-        <v>43227.4444444488</v>
-      </c>
-      <c r="B930" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="931" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A931" s="1" t="n">
-        <v>43227.4513888933</v>
-      </c>
-      <c r="B931" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="932" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A932" s="1" t="n">
-        <v>43227.4583333377</v>
-      </c>
-      <c r="B932" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="933" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A933" s="1" t="n">
-        <v>43227.4652777822</v>
-      </c>
-      <c r="B933" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="934" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A934" s="1" t="n">
-        <v>43227.4722222266</v>
-      </c>
-      <c r="B934" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="935" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A935" s="1" t="n">
-        <v>43227.4791666711</v>
-      </c>
-      <c r="B935" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="936" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A936" s="1" t="n">
-        <v>43227.4861111155</v>
-      </c>
-      <c r="B936" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="937" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A937" s="1" t="n">
-        <v>43227.49305556</v>
-      </c>
-      <c r="B937" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="938" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A938" s="1" t="n">
-        <v>43227.5000000044</v>
-      </c>
-      <c r="B938" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="939" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A939" s="1" t="n">
-        <v>43227.5069444489</v>
-      </c>
-      <c r="B939" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="940" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A940" s="1" t="n">
-        <v>43227.5138888933</v>
-      </c>
-      <c r="B940" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="941" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A941" s="1" t="n">
-        <v>43227.5208333378</v>
-      </c>
-      <c r="B941" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="942" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A942" s="1" t="n">
-        <v>43227.5277777822</v>
-      </c>
-      <c r="B942" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="943" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A943" s="1" t="n">
-        <v>43227.5347222267</v>
-      </c>
-      <c r="B943" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="944" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A944" s="1" t="n">
-        <v>43227.5416666711</v>
-      </c>
-      <c r="B944" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="945" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A945" s="1" t="n">
-        <v>43227.5486111156</v>
-      </c>
-      <c r="B945" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="946" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A946" s="1" t="n">
-        <v>43227.55555556</v>
-      </c>
-      <c r="B946" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="947" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A947" s="1" t="n">
-        <v>43227.5625000045</v>
-      </c>
-      <c r="B947" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="948" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A948" s="1" t="n">
-        <v>43227.5694444489</v>
-      </c>
-      <c r="B948" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="949" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A949" s="1" t="n">
-        <v>43227.5763888934</v>
-      </c>
-      <c r="B949" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="950" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A950" s="1" t="n">
-        <v>43227.5833333378</v>
-      </c>
-      <c r="B950" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="951" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A951" s="1" t="n">
-        <v>43227.5902777823</v>
-      </c>
-      <c r="B951" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="952" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A952" s="1" t="n">
-        <v>43227.5972222267</v>
-      </c>
-      <c r="B952" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="953" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A953" s="1" t="n">
-        <v>43227.6041666712</v>
-      </c>
-      <c r="B953" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="954" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A954" s="1" t="n">
-        <v>43227.6111111156</v>
-      </c>
-      <c r="B954" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="955" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A955" s="1" t="n">
-        <v>43227.6180555601</v>
-      </c>
-      <c r="B955" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="956" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A956" s="1" t="n">
-        <v>43227.6250000045</v>
-      </c>
-      <c r="B956" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="957" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A957" s="1" t="n">
-        <v>43227.631944449</v>
-      </c>
-      <c r="B957" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="958" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A958" s="1" t="n">
-        <v>43227.6388888934</v>
-      </c>
-      <c r="B958" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="959" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A959" s="1" t="n">
-        <v>43227.6458333379</v>
-      </c>
-      <c r="B959" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="960" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A960" s="1" t="n">
-        <v>43227.6527777823</v>
-      </c>
-      <c r="B960" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="961" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A961" s="1" t="n">
-        <v>43227.6597222268</v>
-      </c>
-      <c r="B961" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="962" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A962" s="1" t="n">
-        <v>43227.6666666712</v>
-      </c>
-      <c r="B962" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="963" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A963" s="1" t="n">
-        <v>43227.6736111157</v>
-      </c>
-      <c r="B963" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="964" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A964" s="1" t="n">
-        <v>43227.6805555601</v>
-      </c>
-      <c r="B964" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="965" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A965" s="1" t="n">
-        <v>43227.6875000046</v>
-      </c>
-      <c r="B965" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="966" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A966" s="1" t="n">
-        <v>43227.694444449</v>
-      </c>
-      <c r="B966" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="967" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A967" s="1" t="n">
-        <v>43227.7013888935</v>
-      </c>
-      <c r="B967" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="968" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A968" s="1" t="n">
-        <v>43227.7083333379</v>
-      </c>
-      <c r="B968" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="969" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A969" s="1" t="n">
-        <v>43227.7152777824</v>
-      </c>
-      <c r="B969" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="970" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A970" s="1" t="n">
-        <v>43227.7222222268</v>
-      </c>
-      <c r="B970" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="971" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A971" s="1" t="n">
-        <v>43227.7291666713</v>
-      </c>
-      <c r="B971" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="972" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A972" s="1" t="n">
-        <v>43227.7361111157</v>
-      </c>
-      <c r="B972" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="973" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A973" s="1" t="n">
-        <v>43227.7430555602</v>
-      </c>
-      <c r="B973" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="974" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A974" s="1" t="n">
-        <v>43227.7500000046</v>
-      </c>
-      <c r="B974" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="975" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A975" s="1" t="n">
-        <v>43227.7569444491</v>
-      </c>
-      <c r="B975" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="976" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A976" s="1" t="n">
-        <v>43227.7638888935</v>
-      </c>
-      <c r="B976" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="977" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A977" s="1" t="n">
-        <v>43227.770833338</v>
-      </c>
-      <c r="B977" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="978" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A978" s="1" t="n">
-        <v>43227.7777777824</v>
-      </c>
-      <c r="B978" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="979" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A979" s="1" t="n">
-        <v>43227.7847222269</v>
-      </c>
-      <c r="B979" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="980" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A980" s="1" t="n">
-        <v>43227.7916666713</v>
-      </c>
-      <c r="B980" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="981" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A981" s="1" t="n">
-        <v>43227.7986111158</v>
-      </c>
-      <c r="B981" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="982" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A982" s="1" t="n">
-        <v>43227.8055555602</v>
-      </c>
-      <c r="B982" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="983" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A983" s="1" t="n">
-        <v>43227.8125000047</v>
-      </c>
-      <c r="B983" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="984" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A984" s="1" t="n">
-        <v>43227.8194444491</v>
-      </c>
-      <c r="B984" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="985" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A985" s="1" t="n">
-        <v>43227.8263888936</v>
-      </c>
-      <c r="B985" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="986" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A986" s="1" t="n">
-        <v>43227.833333338</v>
-      </c>
-      <c r="B986" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="987" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A987" s="1" t="n">
-        <v>43227.8402777825</v>
-      </c>
-      <c r="B987" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="988" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A988" s="1" t="n">
-        <v>43227.8472222269</v>
-      </c>
-      <c r="B988" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="989" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A989" s="1" t="n">
-        <v>43227.8541666714</v>
-      </c>
-      <c r="B989" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="990" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A990" s="1" t="n">
-        <v>43227.8611111158</v>
-      </c>
-      <c r="B990" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="991" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A991" s="1" t="n">
-        <v>43227.8680555603</v>
-      </c>
-      <c r="B991" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="992" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A992" s="1" t="n">
-        <v>43227.8750000047</v>
-      </c>
-      <c r="B992" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="993" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A993" s="1" t="n">
-        <v>43227.8819444492</v>
-      </c>
-      <c r="B993" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="994" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A994" s="1" t="n">
-        <v>43227.8888888936</v>
-      </c>
-      <c r="B994" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="995" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A995" s="1" t="n">
-        <v>43227.8958333381</v>
-      </c>
-      <c r="B995" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="996" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A996" s="1" t="n">
-        <v>43227.9027777825</v>
-      </c>
-      <c r="B996" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="997" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A997" s="1" t="n">
-        <v>43227.909722227</v>
-      </c>
-      <c r="B997" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="998" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A998" s="1" t="n">
-        <v>43227.9166666714</v>
-      </c>
-      <c r="B998" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="999" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A999" s="1" t="n">
-        <v>43227.9236111159</v>
-      </c>
-      <c r="B999" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1000" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="1" t="n">
-        <v>43227.9305555603</v>
-      </c>
-      <c r="B1000" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1001" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1001" s="1" t="n">
-        <v>43227.9375000048</v>
-      </c>
-      <c r="B1001" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1002" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1002" s="1" t="n">
-        <v>43227.9444444492</v>
-      </c>
-      <c r="B1002" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1003" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1003" s="1" t="n">
-        <v>43227.9513888937</v>
-      </c>
-      <c r="B1003" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1004" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1004" s="1" t="n">
-        <v>43227.9583333381</v>
-      </c>
-      <c r="B1004" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1005" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1005" s="1" t="n">
-        <v>43227.9652777826</v>
-      </c>
-      <c r="B1005" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1006" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1006" s="1" t="n">
-        <v>43227.972222227</v>
-      </c>
-      <c r="B1006" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1007" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1007" s="1" t="n">
-        <v>43227.9791666715</v>
-      </c>
-      <c r="B1007" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1008" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1008" s="1" t="n">
-        <v>43227.9861111159</v>
-      </c>
-      <c r="B1008" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1009" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1009" s="1" t="n">
-        <v>43227.9930555604</v>
-      </c>
-      <c r="B1009" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1010" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1010" s="1" t="n">
-        <v>43228.0000000048</v>
-      </c>
-      <c r="B1010" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1011" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1011" s="1" t="n">
-        <v>43228.0069444493</v>
-      </c>
-      <c r="B1011" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1012" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1012" s="1" t="n">
-        <v>43228.0138888937</v>
-      </c>
-      <c r="B1012" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1013" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1013" s="1" t="n">
-        <v>43228.0208333382</v>
-      </c>
-      <c r="B1013" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1014" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1014" s="1" t="n">
-        <v>43228.0277777826</v>
-      </c>
-      <c r="B1014" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1015" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1015" s="1" t="n">
-        <v>43228.0347222271</v>
-      </c>
-      <c r="B1015" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1016" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1016" s="1" t="n">
-        <v>43228.0416666715</v>
-      </c>
-      <c r="B1016" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1017" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1017" s="1" t="n">
-        <v>43228.048611116</v>
-      </c>
-      <c r="B1017" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1018" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1018" s="1" t="n">
-        <v>43228.0555555604</v>
-      </c>
-      <c r="B1018" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1019" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1019" s="1" t="n">
-        <v>43228.0625000049</v>
-      </c>
-      <c r="B1019" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1020" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1020" s="1" t="n">
-        <v>43228.0694444493</v>
-      </c>
-      <c r="B1020" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1021" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1021" s="1" t="n">
-        <v>43228.0763888938</v>
-      </c>
-      <c r="B1021" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1022" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1022" s="1" t="n">
-        <v>43228.0833333382</v>
-      </c>
-      <c r="B1022" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1023" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1023" s="1" t="n">
-        <v>43228.0902777827</v>
-      </c>
-      <c r="B1023" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1024" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1024" s="1" t="n">
-        <v>43228.0972222271</v>
-      </c>
-      <c r="B1024" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1025" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1025" s="1" t="n">
-        <v>43228.1041666716</v>
-      </c>
-      <c r="B1025" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1026" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1026" s="1" t="n">
-        <v>43228.111111116</v>
-      </c>
-      <c r="B1026" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1027" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1027" s="1" t="n">
-        <v>43228.1180555605</v>
-      </c>
-      <c r="B1027" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1028" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1028" s="1" t="n">
-        <v>43228.1250000049</v>
-      </c>
-      <c r="B1028" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1029" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1029" s="1" t="n">
-        <v>43228.1319444494</v>
-      </c>
-      <c r="B1029" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1030" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1030" s="1" t="n">
-        <v>43228.1388888938</v>
-      </c>
-      <c r="B1030" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1031" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1031" s="1" t="n">
-        <v>43228.1458333383</v>
-      </c>
-      <c r="B1031" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1032" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1032" s="1" t="n">
-        <v>43228.1527777827</v>
-      </c>
-      <c r="B1032" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1033" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1033" s="1" t="n">
-        <v>43228.1597222272</v>
-      </c>
-      <c r="B1033" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1034" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1034" s="1" t="n">
-        <v>43228.1666666716</v>
-      </c>
-      <c r="B1034" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1035" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1035" s="1" t="n">
-        <v>43228.1736111161</v>
-      </c>
-      <c r="B1035" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1036" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1036" s="1" t="n">
-        <v>43228.1805555605</v>
-      </c>
-      <c r="B1036" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1037" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1037" s="1" t="n">
-        <v>43228.187500005</v>
-      </c>
-      <c r="B1037" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1038" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1038" s="1" t="n">
-        <v>43228.1944444494</v>
-      </c>
-      <c r="B1038" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1039" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1039" s="1" t="n">
-        <v>43228.2013888939</v>
-      </c>
-      <c r="B1039" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1040" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1040" s="1" t="n">
-        <v>43228.2083333383</v>
-      </c>
-      <c r="B1040" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1041" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1041" s="1" t="n">
-        <v>43228.2152777828</v>
-      </c>
-      <c r="B1041" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1042" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1042" s="1" t="n">
-        <v>43228.2222222272</v>
-      </c>
-      <c r="B1042" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1043" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1043" s="1" t="n">
-        <v>43228.2291666717</v>
-      </c>
-      <c r="B1043" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1044" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1044" s="1" t="n">
-        <v>43228.2361111161</v>
-      </c>
-      <c r="B1044" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1045" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1045" s="1" t="n">
-        <v>43228.2430555606</v>
-      </c>
-      <c r="B1045" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1046" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1046" s="1" t="n">
-        <v>43228.250000005</v>
-      </c>
-      <c r="B1046" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1047" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1047" s="1" t="n">
-        <v>43228.2569444495</v>
-      </c>
-      <c r="B1047" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1048" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1048" s="1" t="n">
-        <v>43228.2638888939</v>
-      </c>
-      <c r="B1048" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1049" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1049" s="1" t="n">
-        <v>43228.2708333384</v>
-      </c>
-      <c r="B1049" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1050" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1050" s="1" t="n">
-        <v>43228.2777777828</v>
-      </c>
-      <c r="B1050" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1051" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1051" s="1" t="n">
-        <v>43228.2847222273</v>
-      </c>
-      <c r="B1051" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1052" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1052" s="1" t="n">
-        <v>43228.2916666717</v>
-      </c>
-      <c r="B1052" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1053" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1053" s="1" t="n">
-        <v>43228.2986111162</v>
-      </c>
-      <c r="B1053" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1054" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1054" s="1" t="n">
-        <v>43228.3055555606</v>
-      </c>
-      <c r="B1054" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1055" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1055" s="1" t="n">
-        <v>43228.3125000051</v>
-      </c>
-      <c r="B1055" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1056" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1056" s="1" t="n">
-        <v>43228.3194444495</v>
-      </c>
-      <c r="B1056" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1057" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1057" s="1" t="n">
-        <v>43228.326388894</v>
-      </c>
-      <c r="B1057" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1058" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1058" s="1" t="n">
-        <v>43228.3333333384</v>
-      </c>
-      <c r="B1058" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1059" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1059" s="1" t="n">
-        <v>43228.3402777829</v>
-      </c>
-      <c r="B1059" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1060" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1060" s="1" t="n">
-        <v>43228.3472222273</v>
-      </c>
-      <c r="B1060" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1061" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1061" s="1" t="n">
-        <v>43228.3541666718</v>
-      </c>
-      <c r="B1061" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1062" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1062" s="1" t="n">
-        <v>43228.3611111162</v>
-      </c>
-      <c r="B1062" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1063" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1063" s="1" t="n">
-        <v>43228.3680555607</v>
-      </c>
-      <c r="B1063" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1064" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1064" s="1" t="n">
-        <v>43228.3750000051</v>
-      </c>
-      <c r="B1064" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1065" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1065" s="1" t="n">
-        <v>43228.3819444496</v>
-      </c>
-      <c r="B1065" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1066" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1066" s="1" t="n">
-        <v>43228.388888894</v>
-      </c>
-      <c r="B1066" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1067" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1067" s="1" t="n">
-        <v>43228.3958333385</v>
-      </c>
-      <c r="B1067" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1068" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1068" s="1" t="n">
-        <v>43228.4027777829</v>
-      </c>
-      <c r="B1068" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1069" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1069" s="1" t="n">
-        <v>43228.4097222274</v>
-      </c>
-      <c r="B1069" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1070" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1070" s="1" t="n">
-        <v>43228.4166666718</v>
-      </c>
-      <c r="B1070" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1071" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1071" s="1" t="n">
-        <v>43228.4236111163</v>
-      </c>
-      <c r="B1071" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1072" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1072" s="1" t="n">
-        <v>43228.4305555607</v>
-      </c>
-      <c r="B1072" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1073" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1073" s="1" t="n">
-        <v>43228.4375000052</v>
-      </c>
-      <c r="B1073" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1074" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1074" s="1" t="n">
-        <v>43228.4444444496</v>
-      </c>
-      <c r="B1074" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1075" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1075" s="1" t="n">
-        <v>43228.4513888941</v>
-      </c>
-      <c r="B1075" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1076" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1076" s="1" t="n">
-        <v>43228.4583333385</v>
-      </c>
-      <c r="B1076" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1077" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1077" s="1" t="n">
-        <v>43228.465277783</v>
-      </c>
-      <c r="B1077" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1078" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1078" s="1" t="n">
-        <v>43228.4722222274</v>
-      </c>
-      <c r="B1078" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1079" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1079" s="1" t="n">
-        <v>43228.4791666719</v>
-      </c>
-      <c r="B1079" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1080" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1080" s="1" t="n">
-        <v>43228.4861111163</v>
-      </c>
-      <c r="B1080" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1081" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1081" s="1" t="n">
-        <v>43228.4930555608</v>
-      </c>
-      <c r="B1081" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1082" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1082" s="1" t="n">
-        <v>43228.5000000052</v>
-      </c>
-      <c r="B1082" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1083" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1083" s="1" t="n">
-        <v>43228.5069444497</v>
-      </c>
-      <c r="B1083" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1084" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1084" s="1" t="n">
-        <v>43228.5138888941</v>
-      </c>
-      <c r="B1084" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1085" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1085" s="1" t="n">
-        <v>43228.5208333386</v>
-      </c>
-      <c r="B1085" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1086" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1086" s="1" t="n">
-        <v>43228.527777783</v>
-      </c>
-      <c r="B1086" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1087" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1087" s="1" t="n">
-        <v>43228.5347222275</v>
-      </c>
-      <c r="B1087" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1088" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1088" s="1" t="n">
-        <v>43228.5416666719</v>
-      </c>
-      <c r="B1088" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1089" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1089" s="1" t="n">
-        <v>43228.5486111164</v>
-      </c>
-      <c r="B1089" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1090" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1090" s="1" t="n">
-        <v>43228.5555555608</v>
-      </c>
-      <c r="B1090" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1091" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1091" s="1" t="n">
-        <v>43228.5625000053</v>
-      </c>
-      <c r="B1091" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1092" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1092" s="1" t="n">
-        <v>43228.5694444497</v>
-      </c>
-      <c r="B1092" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1093" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1093" s="1" t="n">
-        <v>43228.5763888942</v>
-      </c>
-      <c r="B1093" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1094" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1094" s="1" t="n">
-        <v>43228.5833333386</v>
-      </c>
-      <c r="B1094" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1095" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1095" s="1" t="n">
-        <v>43228.5902777831</v>
-      </c>
-      <c r="B1095" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1096" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1096" s="1" t="n">
-        <v>43228.5972222275</v>
-      </c>
-      <c r="B1096" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1097" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1097" s="1" t="n">
-        <v>43228.604166672</v>
-      </c>
-      <c r="B1097" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1098" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1098" s="1" t="n">
-        <v>43228.6111111164</v>
-      </c>
-      <c r="B1098" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1099" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1099" s="1" t="n">
-        <v>43228.6180555609</v>
-      </c>
-      <c r="B1099" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1100" s="1" t="n">
-        <v>43228.6250000053</v>
-      </c>
-      <c r="B1100" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1101" s="1" t="n">
-        <v>43228.6319444498</v>
-      </c>
-      <c r="B1101" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1102" s="1" t="n">
-        <v>43228.6388888942</v>
-      </c>
-      <c r="B1102" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1103" s="1" t="n">
-        <v>43228.6458333387</v>
-      </c>
-      <c r="B1103" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1104" s="1" t="n">
-        <v>43228.6527777831</v>
-      </c>
-      <c r="B1104" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1105" s="1" t="n">
-        <v>43228.6597222276</v>
-      </c>
-      <c r="B1105" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1106" s="1" t="n">
-        <v>43228.666666672</v>
-      </c>
-      <c r="B1106" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1107" s="1" t="n">
-        <v>43228.6736111165</v>
-      </c>
-      <c r="B1107" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1108" s="1" t="n">
-        <v>43228.6805555609</v>
-      </c>
-      <c r="B1108" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1109" s="1" t="n">
-        <v>43228.6875000054</v>
-      </c>
-      <c r="B1109" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1110" s="1" t="n">
-        <v>43228.6944444498</v>
-      </c>
-      <c r="B1110" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1111" s="1" t="n">
-        <v>43228.7013888943</v>
-      </c>
-      <c r="B1111" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1112" s="1" t="n">
-        <v>43228.7083333387</v>
-      </c>
-      <c r="B1112" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1113" s="1" t="n">
-        <v>43228.7152777832</v>
-      </c>
-      <c r="B1113" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1114" s="1" t="n">
-        <v>43228.7222222276</v>
-      </c>
-      <c r="B1114" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1115" s="1" t="n">
-        <v>43228.7291666721</v>
-      </c>
-      <c r="B1115" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1116" s="1" t="n">
-        <v>43228.7361111165</v>
-      </c>
-      <c r="B1116" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1117" s="1" t="n">
-        <v>43228.743055561</v>
-      </c>
-      <c r="B1117" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1118" s="1" t="n">
-        <v>43228.7500000054</v>
-      </c>
-      <c r="B1118" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1119" s="1" t="n">
-        <v>43228.7569444499</v>
-      </c>
-      <c r="B1119" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1120" s="1" t="n">
-        <v>43228.7638888943</v>
-      </c>
-      <c r="B1120" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1121" s="1" t="n">
-        <v>43228.7708333388</v>
-      </c>
-      <c r="B1121" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1122" s="1" t="n">
-        <v>43228.7777777832</v>
-      </c>
-      <c r="B1122" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1123" s="1" t="n">
-        <v>43228.7847222277</v>
-      </c>
-      <c r="B1123" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1124" s="1" t="n">
-        <v>43228.7916666721</v>
-      </c>
-      <c r="B1124" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1125" s="1" t="n">
-        <v>43228.7986111166</v>
-      </c>
-      <c r="B1125" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1126" s="1" t="n">
-        <v>43228.805555561</v>
-      </c>
-      <c r="B1126" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1127" s="1" t="n">
-        <v>43228.8125000055</v>
-      </c>
-      <c r="B1127" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1128" s="1" t="n">
-        <v>43228.8194444499</v>
-      </c>
-      <c r="B1128" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1129" s="1" t="n">
-        <v>43228.8263888944</v>
-      </c>
-      <c r="B1129" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1130" s="1" t="n">
-        <v>43228.8333333388</v>
-      </c>
-      <c r="B1130" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1131" s="1" t="n">
-        <v>43228.8402777833</v>
-      </c>
-      <c r="B1131" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1132" s="1" t="n">
-        <v>43228.8472222277</v>
-      </c>
-      <c r="B1132" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1133" s="1" t="n">
-        <v>43228.8541666722</v>
-      </c>
-      <c r="B1133" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1134" s="1" t="n">
-        <v>43228.8611111166</v>
-      </c>
-      <c r="B1134" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1135" s="1" t="n">
-        <v>43228.8680555611</v>
-      </c>
-      <c r="B1135" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1136" s="1" t="n">
-        <v>43228.8750000055</v>
-      </c>
-      <c r="B1136" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1137" s="1" t="n">
-        <v>43228.88194445</v>
-      </c>
-      <c r="B1137" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1138" s="1" t="n">
-        <v>43228.8888888944</v>
-      </c>
-      <c r="B1138" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1139" s="1" t="n">
-        <v>43228.8958333389</v>
-      </c>
-      <c r="B1139" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1140" s="1" t="n">
-        <v>43228.9027777833</v>
-      </c>
-      <c r="B1140" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1141" s="1" t="n">
-        <v>43228.9097222278</v>
-      </c>
-      <c r="B1141" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1142" s="1" t="n">
-        <v>43228.9166666722</v>
-      </c>
-      <c r="B1142" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1143" s="1" t="n">
-        <v>43228.9236111167</v>
-      </c>
-      <c r="B1143" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1144" s="1" t="n">
-        <v>43228.9305555611</v>
-      </c>
-      <c r="B1144" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1145" s="1" t="n">
-        <v>43228.9375000056</v>
-      </c>
-      <c r="B1145" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1146" s="1" t="n">
-        <v>43228.94444445</v>
-      </c>
-      <c r="B1146" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1147" s="1" t="n">
-        <v>43228.9513888945</v>
-      </c>
-      <c r="B1147" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1148" s="1" t="n">
-        <v>43228.9583333389</v>
-      </c>
-      <c r="B1148" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1149" s="1" t="n">
-        <v>43228.9652777834</v>
-      </c>
-      <c r="B1149" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1150" s="1" t="n">
-        <v>43228.9722222278</v>
-      </c>
-      <c r="B1150" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1151" s="1" t="n">
-        <v>43228.9791666723</v>
-      </c>
-      <c r="B1151" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1152" s="1" t="n">
-        <v>43228.9861111167</v>
-      </c>
-      <c r="B1152" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="1153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1153" s="1" t="n">
-        <v>43228.9930555612</v>
-      </c>
-      <c r="B1153" s="0" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
+    <row r="722" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1000" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1002" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1004" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1005" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1006" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1007" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1008" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1009" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1010" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1011" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1012" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1013" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1014" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1015" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1016" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1017" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1018" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1019" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1020" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1021" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1022" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1023" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1024" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1025" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1026" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1027" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1028" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1029" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1030" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1031" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1032" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1033" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1034" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1035" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1036" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1037" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1038" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1039" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1040" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1041" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1042" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1043" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1044" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1045" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1049" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1050" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1051" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1052" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1053" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1054" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1055" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1056" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1057" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1058" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1059" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1060" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1061" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1062" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1063" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1064" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1065" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1066" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1067" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1068" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1069" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1070" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1071" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1072" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1073" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1074" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1075" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1076" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1077" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1078" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1079" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1080" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1081" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1082" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1083" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1084" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1085" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1086" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1087" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1088" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1089" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1090" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1091" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1092" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1093" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1094" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1095" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1096" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1097" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1098" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1099" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>